<commit_message>
Added Excel read TC
</commit_message>
<xml_diff>
--- a/src/test/resources/environment/QA/TestData/TestData.xlsx
+++ b/src/test/resources/environment/QA/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suraj/Documents/GitHub/SeleniumTestNG/src/test/resources/environment/UAT/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suraj_shivajisalunkh\testautomationproject\src\test\resources\environment\QA\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F03B533-A036-AA44-8CC0-B5B256EDE09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C520DDA-2033-47EE-9BF8-78F5BD06E250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,28 +36,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>isLoginSuccessful</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Logged In Successfully</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Your username is invalid!</t>
+  </si>
+  <si>
+    <t>Test@123</t>
+  </si>
+  <si>
+    <t>Your password is invalid!</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -67,14 +92,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,79 +129,23 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -465,93 +427,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.08984375" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="38.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="11"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="11"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="12"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="12"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="13"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="13"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="12"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="12"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>